<commit_message>
Added courtyard clearing to glyphs for overlay symbols
</commit_message>
<xml_diff>
--- a/keyboards/handwired/polykybd/split72/keymaps/default/lang/lang_lut.xlsx
+++ b/keyboards/handwired/polykybd/split72/keymaps/default/lang/lang_lut.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2892" uniqueCount="1417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2904" uniqueCount="1417">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -5351,7 +5351,7 @@
       <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.25390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="39.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="15.74"/>
@@ -28384,11 +28384,11 @@
   <dimension ref="A1:CC69"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="T23" activeCellId="0" sqref="T23"/>
+      <selection pane="topRight" activeCell="U1" activeCellId="0" sqref="U1"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="AE41" activeCellId="0" sqref="AE41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31935,9 +31935,15 @@
       <c r="AC28" s="94" t="s">
         <v>1112</v>
       </c>
-      <c r="AD28" s="95"/>
-      <c r="AE28" s="95"/>
-      <c r="AF28" s="95"/>
+      <c r="AD28" s="95" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE28" s="95" t="s">
+        <v>1109</v>
+      </c>
+      <c r="AF28" s="95" t="n">
+        <v>1</v>
+      </c>
       <c r="AG28" s="95"/>
       <c r="AH28" s="96" t="s">
         <v>678</v>
@@ -32134,9 +32140,15 @@
       <c r="AC29" s="123" t="s">
         <v>49</v>
       </c>
-      <c r="AD29" s="95"/>
-      <c r="AE29" s="95"/>
-      <c r="AF29" s="95"/>
+      <c r="AD29" s="95" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE29" s="95" t="s">
+        <v>1072</v>
+      </c>
+      <c r="AF29" s="95" t="n">
+        <v>2</v>
+      </c>
       <c r="AG29" s="95"/>
       <c r="AH29" s="96" t="s">
         <v>691</v>
@@ -32335,9 +32347,15 @@
       <c r="AC30" s="94" t="s">
         <v>1116</v>
       </c>
-      <c r="AD30" s="95"/>
-      <c r="AE30" s="95"/>
-      <c r="AF30" s="95"/>
+      <c r="AD30" s="95" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE30" s="95" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AF30" s="95" t="n">
+        <v>3</v>
+      </c>
       <c r="AG30" s="95"/>
       <c r="AH30" s="96" t="s">
         <v>622</v>
@@ -32528,9 +32546,15 @@
       <c r="AC31" s="94" t="s">
         <v>1121</v>
       </c>
-      <c r="AD31" s="95"/>
-      <c r="AE31" s="95"/>
-      <c r="AF31" s="95"/>
+      <c r="AD31" s="95" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE31" s="95" t="s">
+        <v>1121</v>
+      </c>
+      <c r="AF31" s="95" t="n">
+        <v>4</v>
+      </c>
       <c r="AG31" s="95"/>
       <c r="AH31" s="96" t="s">
         <v>626</v>
@@ -32723,9 +32747,15 @@
       <c r="AC32" s="123" t="s">
         <v>98</v>
       </c>
-      <c r="AD32" s="95"/>
-      <c r="AE32" s="95"/>
-      <c r="AF32" s="95"/>
+      <c r="AD32" s="95" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE32" s="95" t="s">
+        <v>1126</v>
+      </c>
+      <c r="AF32" s="95" t="n">
+        <v>5</v>
+      </c>
       <c r="AG32" s="95"/>
       <c r="AH32" s="96" t="s">
         <v>628</v>
@@ -32920,9 +32950,15 @@
         <v>6</v>
       </c>
       <c r="AC33" s="94"/>
-      <c r="AD33" s="95"/>
-      <c r="AE33" s="95"/>
-      <c r="AF33" s="95"/>
+      <c r="AD33" s="95" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE33" s="95" t="s">
+        <v>1118</v>
+      </c>
+      <c r="AF33" s="95" t="n">
+        <v>6</v>
+      </c>
       <c r="AG33" s="95"/>
       <c r="AH33" s="96" t="s">
         <v>630</v>
@@ -33121,9 +33157,15 @@
       <c r="AC34" s="94" t="s">
         <v>1019</v>
       </c>
-      <c r="AD34" s="95"/>
-      <c r="AE34" s="95"/>
-      <c r="AF34" s="95"/>
+      <c r="AD34" s="95" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE34" s="95" t="s">
+        <v>1110</v>
+      </c>
+      <c r="AF34" s="95" t="n">
+        <v>7</v>
+      </c>
       <c r="AG34" s="95"/>
       <c r="AH34" s="96" t="s">
         <v>712</v>
@@ -33320,9 +33362,15 @@
       <c r="AC35" s="94" t="s">
         <v>1035</v>
       </c>
-      <c r="AD35" s="95"/>
-      <c r="AE35" s="95"/>
-      <c r="AF35" s="95"/>
+      <c r="AD35" s="95" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE35" s="95" t="s">
+        <v>1136</v>
+      </c>
+      <c r="AF35" s="95" t="n">
+        <v>8</v>
+      </c>
       <c r="AG35" s="95"/>
       <c r="AH35" s="96" t="s">
         <v>714</v>
@@ -33519,9 +33567,15 @@
       <c r="AC36" s="94" t="s">
         <v>1026</v>
       </c>
-      <c r="AD36" s="95"/>
-      <c r="AE36" s="95"/>
-      <c r="AF36" s="95"/>
+      <c r="AD36" s="95" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE36" s="95" t="s">
+        <v>1127</v>
+      </c>
+      <c r="AF36" s="95" t="n">
+        <v>9</v>
+      </c>
       <c r="AG36" s="95"/>
       <c r="AH36" s="96" t="s">
         <v>716</v>
@@ -33718,9 +33772,15 @@
       <c r="AC37" s="94" t="s">
         <v>1064</v>
       </c>
-      <c r="AD37" s="95"/>
-      <c r="AE37" s="95"/>
-      <c r="AF37" s="95"/>
+      <c r="AD37" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE37" s="95" t="s">
+        <v>1138</v>
+      </c>
+      <c r="AF37" s="95" t="s">
+        <v>12</v>
+      </c>
       <c r="AG37" s="95"/>
       <c r="AH37" s="96" t="s">
         <v>728</v>
@@ -36609,7 +36669,7 @@
       <c r="AG56" s="140"/>
       <c r="AH56" s="141"/>
       <c r="AI56" s="141" t="n">
-        <v>35</v>
+        <v>-1</v>
       </c>
       <c r="AJ56" s="141"/>
       <c r="AK56" s="141"/>
@@ -36768,7 +36828,7 @@
       <c r="AG57" s="140"/>
       <c r="AH57" s="141"/>
       <c r="AI57" s="141" t="n">
-        <v>15</v>
+        <v>-1</v>
       </c>
       <c r="AJ57" s="141"/>
       <c r="AK57" s="141"/>
@@ -37086,7 +37146,7 @@
       <c r="AG59" s="140"/>
       <c r="AH59" s="141"/>
       <c r="AI59" s="141" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AJ59" s="141"/>
       <c r="AK59" s="141"/>
@@ -37404,7 +37464,7 @@
       <c r="AG61" s="140"/>
       <c r="AH61" s="141"/>
       <c r="AI61" s="141" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AJ61" s="141"/>
       <c r="AK61" s="141"/>
@@ -38474,7 +38534,7 @@
       <selection pane="topLeft" activeCell="O82" activeCellId="0" sqref="O82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="161" width="11.52"/>
   </cols>

</xml_diff>